<commit_message>
Added a date check to catch when new fastq are added to an Experiment for old samples.
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB1EF7-AD86-B448-BF92-48DE57D6FC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4572B57-76A1-C54E-99F4-ED56264E8432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Human</t>
   </si>
@@ -83,18 +83,9 @@
     <t>Illumina RNA Exome Library Prep</t>
   </si>
   <si>
-    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection; NEBNext Ultra II Directional RNA Library Prep with Globin and rRNA Depletion Kit (human,mouse,rat); Illumina Total RNA Prep with RiboZero Plus</t>
-  </si>
-  <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/human_reverse_nextera_rnaAlignQC.yaml</t>
   </si>
   <si>
-    <t>Active Motif ATAC-seq; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (1-plex enrichment); IDT xGEN Human Exome v2 with Nextera Flex Library Prep (4-plex enrichment); ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI</t>
-  </si>
-  <si>
-    <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI</t>
-  </si>
-  <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Config/mouse_gem_cellRanger.yaml</t>
   </si>
   <si>
@@ -122,10 +113,40 @@
     <t># DNASeq</t>
   </si>
   <si>
-    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation; 10x Genomics Chromium Next GEM Single Cell 3' v3.1 Gene Expression Library Preparation</t>
-  </si>
-  <si>
     <t>--config /home/tomatosrvs/AutoAnalysis/autoAnalysis.multiqc.config.yaml</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection; NEBNext Ultra II Directional RNA Library Prep with Globin and rRNA Depletion Kit (human,mouse,rat); Illumina Total RNA Prep with RiboZero Plus; NEBNext Single Cell/Low Input RNA Library Prep</t>
+  </si>
+  <si>
+    <t>Zebrafish</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/zebrafish_reverse_truseq_rnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>NEB Next UltraII Directional RNA Library Prep with poly(A) mRNA Isolation; NEB Next UltraII Directional RNA Library Prep with rRNA Depletion Kit(Zebrafish)</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/rat_reverse_truseq_rnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI; NEBNext Ultra II DNA Library Prep for FFPE DNA</t>
+  </si>
+  <si>
+    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation; 10x Genomics Chromium Next GEM Single Cell 3' v3.1 Gene Expression Library Preparation; 10x Genomics Chromium GEM-X Single Cell 5' v3 Gene Expression, Labor Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation; 10x Genomics Chromium Next GEM Single Cell 3' v3.1 Gene Expression Library Preparation; 10x Genomics Chromium GEM-X Single Cell 5' v3 Gene Expression, Labor Only; </t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (1-plex enrichment); IDT xGEN Human Exome v2 with Nextera Flex Library Prep (4-plex enrichment); ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (3-plex enrichment); NEBNext Ultra II DNA Library Prep for FFPE DNA; Agilent SureSelect Human All Exon v8 with NEB Library Prep for FFPE DNA (2-plex enrichment)</t>
+  </si>
+  <si>
+    <t>NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation</t>
   </si>
 </sst>
 </file>
@@ -542,11 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1575BC-6DBD-9743-ACB5-EE787B21782E}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +618,7 @@
     </row>
     <row r="5" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -608,13 +629,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
@@ -622,13 +643,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -639,129 +660,157 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="D14" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="D12" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+      <c r="D19" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B7">

</xml_diff>